<commit_message>
BackLog arrumado, agora sim
</commit_message>
<xml_diff>
--- a/Documentações/backlog_burndown_grupo_10.xlsx
+++ b/Documentações/backlog_burndown_grupo_10.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
-  <workbookPr defaultThemeVersion="202300"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Renan\Desktop\repositorio\Gas_Busters\Documentações\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D22C25FE-7DCE-4BFB-95CA-7B2EE06847A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{A3CC8B60-91E8-4DBA-95FB-4AC8B4BD430D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$C$1:$C$43</definedName>
+  </definedNames>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="123">
   <si>
     <t>Matéria</t>
   </si>
@@ -399,13 +401,19 @@
   </si>
   <si>
     <t>MEMBROS - GRUPO 10</t>
+  </si>
+  <si>
+    <t>Fazer Slides</t>
+  </si>
+  <si>
+    <t>Fazer os slides para a apresentação da segunda sprint</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -519,7 +527,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -557,11 +565,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -608,19 +642,60 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFE06666"/>
       <color rgb="FF33CC33"/>
       <color rgb="FF0066FF"/>
       <color rgb="FF93C47D"/>
       <color rgb="FF00B050"/>
-      <color rgb="FFE06666"/>
       <color rgb="FFFFD966"/>
       <color rgb="FFC27BA0"/>
     </mruColors>
@@ -637,7 +712,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="pt-BR"/>
   <c:roundedCorners val="0"/>
@@ -676,6 +751,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -782,8 +858,9 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -843,7 +920,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-2700-4359-A6AD-371FAC752817}"/>
             </c:ext>
@@ -920,8 +997,9 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -981,7 +1059,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-2700-4359-A6AD-371FAC752817}"/>
             </c:ext>
@@ -998,11 +1076,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="608668416"/>
-        <c:axId val="608668776"/>
+        <c:axId val="330285880"/>
+        <c:axId val="330323168"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="608668416"/>
+        <c:axId val="330285880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1045,7 +1123,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="608668776"/>
+        <c:crossAx val="330323168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1053,7 +1131,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="608668776"/>
+        <c:axId val="330323168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1089,7 +1167,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="608668416"/>
+        <c:crossAx val="330285880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1103,6 +1181,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -1139,14 +1218,14 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:gradFill flip="none" rotWithShape="1">
@@ -1825,7 +1904,7 @@
         <xdr:cNvPr id="7" name="Gráfico 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4992053-6878-072A-6615-567D8CD2C280}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E4992053-6878-072A-6615-567D8CD2C280}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2162,32 +2241,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14FEDA83-7BC7-418D-998D-DF8955E4369B}">
-  <dimension ref="A1:Q42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:Q43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.375" customWidth="1"/>
     <col min="4" max="4" width="41" customWidth="1"/>
-    <col min="5" max="5" width="91.140625" customWidth="1"/>
-    <col min="6" max="6" width="20.5703125" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="91.125" customWidth="1"/>
+    <col min="6" max="6" width="20.625" customWidth="1"/>
+    <col min="7" max="7" width="12.125" customWidth="1"/>
+    <col min="8" max="8" width="12.75" customWidth="1"/>
     <col min="9" max="9" width="16" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" customWidth="1"/>
+    <col min="10" max="10" width="15.375" customWidth="1"/>
     <col min="11" max="11" width="15" customWidth="1"/>
-    <col min="12" max="12" width="20.42578125" customWidth="1"/>
-    <col min="15" max="15" width="12.140625" customWidth="1"/>
+    <col min="12" max="12" width="20.375" customWidth="1"/>
+    <col min="15" max="15" width="12.125" customWidth="1"/>
     <col min="16" max="16" width="13" customWidth="1"/>
-    <col min="17" max="17" width="12.7109375" customWidth="1"/>
+    <col min="17" max="17" width="12.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="30" customHeight="1">
       <c r="A1" s="14" t="s">
         <v>120</v>
       </c>
@@ -2222,7 +2302,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="18">
       <c r="A2" s="15" t="s">
         <v>115</v>
       </c>
@@ -2266,7 +2346,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="18">
       <c r="A3" s="15" t="s">
         <v>116</v>
       </c>
@@ -2310,7 +2390,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="18">
       <c r="A4" s="15" t="s">
         <v>117</v>
       </c>
@@ -2354,7 +2434,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="18">
       <c r="A5" s="15" t="s">
         <v>118</v>
       </c>
@@ -2398,7 +2478,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="18">
       <c r="A6" s="15" t="s">
         <v>119</v>
       </c>
@@ -2442,7 +2522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17">
       <c r="C7" s="6" t="s">
         <v>12</v>
       </c>
@@ -2474,7 +2554,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17">
       <c r="C8" s="6" t="s">
         <v>12</v>
       </c>
@@ -2506,7 +2586,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17">
       <c r="C9" s="6" t="s">
         <v>14</v>
       </c>
@@ -2538,7 +2618,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17">
       <c r="C10" s="6" t="s">
         <v>14</v>
       </c>
@@ -2570,7 +2650,8 @@
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17">
+      <c r="A11" s="27"/>
       <c r="C11" s="6" t="s">
         <v>14</v>
       </c>
@@ -2602,7 +2683,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17">
       <c r="C12" s="6" t="s">
         <v>14</v>
       </c>
@@ -2634,7 +2715,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17">
       <c r="C13" s="6" t="s">
         <v>14</v>
       </c>
@@ -2666,7 +2747,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17">
       <c r="C14" s="6" t="s">
         <v>14</v>
       </c>
@@ -2698,7 +2779,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17">
       <c r="C15" s="6" t="s">
         <v>14</v>
       </c>
@@ -2730,7 +2811,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17">
       <c r="C16" s="6" t="s">
         <v>14</v>
       </c>
@@ -2762,7 +2843,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:12">
       <c r="C17" s="6" t="s">
         <v>14</v>
       </c>
@@ -2794,7 +2875,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="18" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:12">
       <c r="C18" s="6" t="s">
         <v>13</v>
       </c>
@@ -2826,7 +2907,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="19" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:12">
       <c r="C19" s="6" t="s">
         <v>13</v>
       </c>
@@ -2858,7 +2939,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="20" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:12">
       <c r="C20" s="6" t="s">
         <v>13</v>
       </c>
@@ -2890,7 +2971,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="21" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:12">
       <c r="C21" s="6" t="s">
         <v>13</v>
       </c>
@@ -2922,7 +3003,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="22" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:12">
       <c r="C22" s="6" t="s">
         <v>13</v>
       </c>
@@ -2954,7 +3035,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="23" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:12">
       <c r="C23" s="6" t="s">
         <v>10</v>
       </c>
@@ -2986,7 +3067,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:12">
       <c r="C24" s="6" t="s">
         <v>10</v>
       </c>
@@ -3018,7 +3099,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:12">
       <c r="C25" s="6" t="s">
         <v>10</v>
       </c>
@@ -3050,7 +3131,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="26" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:12">
       <c r="C26" s="6" t="s">
         <v>10</v>
       </c>
@@ -3082,7 +3163,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="27" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:12">
       <c r="C27" s="6" t="s">
         <v>10</v>
       </c>
@@ -3114,7 +3195,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="28" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:12">
       <c r="C28" s="6" t="s">
         <v>10</v>
       </c>
@@ -3146,7 +3227,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="29" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:12">
       <c r="C29" s="6" t="s">
         <v>10</v>
       </c>
@@ -3178,7 +3259,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="30" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:12">
       <c r="C30" s="6" t="s">
         <v>10</v>
       </c>
@@ -3210,7 +3291,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="31" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:12">
       <c r="C31" s="6" t="s">
         <v>10</v>
       </c>
@@ -3242,27 +3323,27 @@
         <v>106</v>
       </c>
     </row>
-    <row r="32" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C32" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D32" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="E32" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="F32" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="G32" s="6">
-        <v>2</v>
-      </c>
-      <c r="H32" s="10" t="s">
+    <row r="32" spans="3:12">
+      <c r="C32" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E32" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="F32" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="G32" s="22">
+        <v>3</v>
+      </c>
+      <c r="H32" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="I32" s="6">
-        <v>3</v>
+      <c r="I32" s="22">
+        <v>1</v>
       </c>
       <c r="J32" s="2" t="s">
         <v>100</v>
@@ -3270,19 +3351,19 @@
       <c r="K32" s="2">
         <v>5</v>
       </c>
-      <c r="L32" s="6" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="33" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="L32" s="22" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="33" spans="3:12">
       <c r="C33" s="6" t="s">
         <v>15</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>82</v>
+        <v>45</v>
       </c>
       <c r="F33" s="7" t="s">
         <v>92</v>
@@ -3294,7 +3375,7 @@
         <v>96</v>
       </c>
       <c r="I33" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J33" s="2" t="s">
         <v>100</v>
@@ -3306,53 +3387,53 @@
         <v>103</v>
       </c>
     </row>
-    <row r="34" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:12">
       <c r="C34" s="6" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F34" s="7" t="s">
         <v>92</v>
       </c>
       <c r="G34" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H34" s="10" t="s">
         <v>96</v>
       </c>
       <c r="I34" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="K34" s="4">
-        <v>21</v>
+        <v>100</v>
+      </c>
+      <c r="K34" s="2">
+        <v>5</v>
       </c>
       <c r="L34" s="6" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="35" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:12">
       <c r="C35" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="F35" s="9" t="s">
-        <v>93</v>
+        <v>84</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>92</v>
       </c>
       <c r="G35" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H35" s="10" t="s">
         <v>96</v>
@@ -3361,187 +3442,187 @@
         <v>3</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="K35" s="2">
-        <v>8</v>
+        <v>101</v>
+      </c>
+      <c r="K35" s="4">
+        <v>21</v>
       </c>
       <c r="L35" s="6" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="36" spans="3:12" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="36" spans="3:12">
       <c r="C36" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F36" s="7" t="s">
-        <v>92</v>
+        <v>68</v>
+      </c>
+      <c r="F36" s="9" t="s">
+        <v>93</v>
       </c>
       <c r="G36" s="6">
-        <v>1</v>
-      </c>
-      <c r="H36" s="8" t="s">
-        <v>95</v>
+        <v>2</v>
+      </c>
+      <c r="H36" s="10" t="s">
+        <v>96</v>
       </c>
       <c r="I36" s="6">
-        <v>1</v>
-      </c>
-      <c r="J36" s="3" t="s">
-        <v>99</v>
+        <v>3</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="K36" s="2">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="L36" s="6" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="37" spans="3:12" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="37" spans="3:12">
       <c r="C37" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E37" s="11" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="F37" s="7" t="s">
         <v>92</v>
       </c>
       <c r="G37" s="6">
-        <v>2</v>
-      </c>
-      <c r="H37" s="10" t="s">
-        <v>96</v>
+        <v>1</v>
+      </c>
+      <c r="H37" s="8" t="s">
+        <v>95</v>
       </c>
       <c r="I37" s="6">
-        <v>2</v>
-      </c>
-      <c r="J37" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J37" s="3" t="s">
         <v>99</v>
       </c>
       <c r="K37" s="2">
         <v>13</v>
       </c>
       <c r="L37" s="6" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="38" spans="3:12" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="38" spans="3:12">
       <c r="C38" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F38" s="7" t="s">
         <v>92</v>
       </c>
       <c r="G38" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H38" s="10" t="s">
         <v>96</v>
       </c>
       <c r="I38" s="6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J38" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="K38" s="4">
+      <c r="K38" s="2">
         <v>13</v>
       </c>
       <c r="L38" s="6" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="39" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:12">
       <c r="C39" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>27</v>
+        <v>85</v>
       </c>
       <c r="F39" s="7" t="s">
         <v>92</v>
       </c>
       <c r="G39" s="6">
-        <v>1</v>
-      </c>
-      <c r="H39" s="8" t="s">
-        <v>95</v>
+        <v>3</v>
+      </c>
+      <c r="H39" s="10" t="s">
+        <v>96</v>
       </c>
       <c r="I39" s="6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="K39" s="2">
-        <v>5</v>
+        <v>99</v>
+      </c>
+      <c r="K39" s="4">
+        <v>13</v>
       </c>
       <c r="L39" s="6" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="40" spans="3:12" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="40" spans="3:12">
       <c r="C40" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="F40" s="8" t="s">
-        <v>94</v>
+        <v>27</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>92</v>
       </c>
       <c r="G40" s="6">
-        <v>2</v>
-      </c>
-      <c r="H40" s="10" t="s">
-        <v>96</v>
+        <v>1</v>
+      </c>
+      <c r="H40" s="8" t="s">
+        <v>95</v>
       </c>
       <c r="I40" s="6">
         <v>1</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K40" s="2">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="L40" s="6" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="41" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:12">
       <c r="C41" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="E41" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="F41" s="7" t="s">
-        <v>92</v>
+        <v>69</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>94</v>
       </c>
       <c r="G41" s="6">
         <v>2</v>
@@ -3553,52 +3634,93 @@
         <v>1</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K41" s="2">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="L41" s="6" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="42" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C42" s="6" t="s">
+    <row r="42" spans="3:12">
+      <c r="C42" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="D42" s="11" t="s">
+      <c r="D42" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="E42" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="F42" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="G42" s="16">
+        <v>2</v>
+      </c>
+      <c r="H42" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="I42" s="16">
+        <v>1</v>
+      </c>
+      <c r="J42" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="K42" s="20">
+        <v>5</v>
+      </c>
+      <c r="L42" s="16" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="43" spans="3:12">
+      <c r="C43" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D43" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="E42" s="11" t="s">
+      <c r="E43" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="F42" s="7" t="s">
+      <c r="F43" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="G42" s="6">
+      <c r="G43" s="6">
         <v>3</v>
       </c>
-      <c r="H42" s="10" t="s">
+      <c r="H43" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="I42" s="6">
+      <c r="I43" s="6">
         <v>3</v>
       </c>
-      <c r="J42" s="2" t="s">
+      <c r="J43" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="K42" s="4">
+      <c r="K43" s="26">
         <v>21</v>
       </c>
-      <c r="L42" s="6" t="s">
+      <c r="L43" s="6" t="s">
         <v>106</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C2:L46">
+  <autoFilter ref="C1:C43">
+    <filterColumn colId="0">
+      <colorFilter dxfId="0"/>
+    </filterColumn>
+    <sortState ref="C2:L43">
+      <sortCondition ref="C1:C43"/>
+    </sortState>
+  </autoFilter>
+  <sortState ref="C2:L46">
     <sortCondition ref="C1:C46"/>
   </sortState>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>